<commit_message>
Add funcionality to create new Household and new Visit (further details will be handle in next commits)
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/household_form.xlsx
+++ b/app/src/main/res/raw/household_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11895" tabRatio="500"/>
+    <workbookView windowWidth="30720" windowHeight="13512" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
   <si>
     <t>group</t>
   </si>
@@ -51,7 +51,7 @@
     <t>readonly</t>
   </si>
   <si>
-    <t>skip_condition</t>
+    <t>display_condition</t>
   </si>
   <si>
     <t>header</t>
@@ -105,6 +105,9 @@
     <t>1.5. Código do Chefe de Agregado</t>
   </si>
   <si>
+    <t>${householdName}='PAUL'</t>
+  </si>
+  <si>
     <t>headName</t>
   </si>
   <si>
@@ -148,6 +151,15 @@
   </si>
   <si>
     <t>1.9. Data da Visita</t>
+  </si>
+  <si>
+    <t>modules</t>
+  </si>
+  <si>
+    <t>Access Granted to Modules</t>
+  </si>
+  <si>
+    <t>Acesso permitido ao Módulos</t>
   </si>
   <si>
     <t>value</t>
@@ -177,9 +189,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -201,6 +213,112 @@
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -212,131 +330,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -349,43 +361,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -397,139 +523,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -543,35 +555,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -606,11 +594,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -622,6 +616,15 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -640,145 +643,154 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="8" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="7" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -788,10 +800,13 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
@@ -1113,22 +1128,22 @@
   <sheetPr/>
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13.2"/>
   <cols>
-    <col min="2" max="2" width="11.1428571428571" customWidth="true"/>
-    <col min="3" max="3" width="14.1428571428571" customWidth="true"/>
-    <col min="4" max="4" width="20.1428571428571" customWidth="true"/>
-    <col min="5" max="5" width="11.7142857142857" customWidth="true"/>
-    <col min="6" max="6" width="9.71428571428571" customWidth="true"/>
-    <col min="7" max="7" width="26.8571428571429" customWidth="true"/>
-    <col min="8" max="8" width="32.4285714285714" customWidth="true"/>
-    <col min="9" max="9" width="21.7142857142857" customWidth="true"/>
-    <col min="10" max="10" width="9.28571428571429" customWidth="true"/>
-    <col min="12" max="12" width="13.8571428571429" customWidth="true"/>
+    <col min="2" max="2" width="11.1388888888889" customWidth="true"/>
+    <col min="3" max="3" width="14.1388888888889" customWidth="true"/>
+    <col min="4" max="4" width="20.1388888888889" customWidth="true"/>
+    <col min="5" max="5" width="11.712962962963" customWidth="true"/>
+    <col min="6" max="6" width="9.71296296296296" customWidth="true"/>
+    <col min="7" max="7" width="44.712962962963" customWidth="true"/>
+    <col min="8" max="8" width="32.4259259259259" customWidth="true"/>
+    <col min="9" max="9" width="21.712962962963" customWidth="true"/>
+    <col min="10" max="10" width="9.28703703703704" customWidth="true"/>
+    <col min="12" max="12" width="22.9444444444444" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1165,7 +1180,7 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1185,7 +1200,7 @@
       <c r="H2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="2"/>
+      <c r="I2" s="3"/>
       <c r="J2" t="b">
         <v>1</v>
       </c>
@@ -1209,7 +1224,7 @@
       <c r="H3" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="2"/>
+      <c r="I3" s="3"/>
       <c r="J3" t="b">
         <v>1</v>
       </c>
@@ -1233,7 +1248,7 @@
       <c r="H4" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="2"/>
+      <c r="I4" s="3"/>
       <c r="J4" t="b">
         <v>1</v>
       </c>
@@ -1255,12 +1270,12 @@
       <c r="H5" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="2"/>
+      <c r="I5" s="3"/>
       <c r="J5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:12">
       <c r="A6" s="1"/>
       <c r="D6" t="s">
         <v>26</v>
@@ -1274,68 +1289,74 @@
       <c r="H6" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="2"/>
+      <c r="I6" s="3"/>
       <c r="K6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="L6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="1"/>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="I7" s="3"/>
       <c r="K7" t="b">
         <v>1</v>
+      </c>
+      <c r="L7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1"/>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="I8" s="3"/>
       <c r="J8" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H9" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="I9" s="3"/>
       <c r="J9" t="b">
         <v>1</v>
       </c>
@@ -1345,21 +1366,21 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H10" t="s">
-        <v>43</v>
-      </c>
-      <c r="I10" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="I10" s="3"/>
       <c r="J10" t="b">
         <v>1</v>
       </c>
@@ -1367,21 +1388,41 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="1"/>
-      <c r="I11" s="2"/>
+    <row r="11" spans="1:11">
+      <c r="A11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1"/>
-      <c r="I12" s="2"/>
+      <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1"/>
-      <c r="I13" s="2"/>
+      <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1"/>
-      <c r="I14" s="3"/>
+      <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="1"/>
@@ -1435,10 +1476,10 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="13.2" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="true"/>
-    <col min="2" max="2" width="12.2857142857143" customWidth="true"/>
+    <col min="2" max="2" width="12.287037037037" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1446,7 +1487,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
@@ -1470,33 +1511,33 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="13.2" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="true"/>
-    <col min="2" max="2" width="20.4285714285714" customWidth="true"/>
-    <col min="3" max="3" width="23.2857142857143" customWidth="true"/>
+    <col min="2" max="2" width="20.4259259259259" customWidth="true"/>
+    <col min="3" max="3" width="23.287037037037" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add checks on VisitFormUtil and fixes some bugs
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/household_form.xlsx
+++ b/app/src/main/res/raw/household_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30720" windowHeight="13512" tabRatio="500"/>
+    <workbookView windowWidth="20940" windowHeight="11595" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
   <si>
     <t>group</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>1.5. Código do Chefe de Agregado</t>
-  </si>
-  <si>
-    <t>${householdName}='PAUL'</t>
   </si>
   <si>
     <t>headName</t>
@@ -188,9 +185,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -201,18 +198,100 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -224,99 +303,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -331,22 +320,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -361,187 +358,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -580,6 +577,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -590,6 +602,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -611,6 +632,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -619,184 +649,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="7" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1128,22 +1125,22 @@
   <sheetPr/>
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6:L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="11.1388888888889" customWidth="true"/>
-    <col min="3" max="3" width="14.1388888888889" customWidth="true"/>
-    <col min="4" max="4" width="20.1388888888889" customWidth="true"/>
-    <col min="5" max="5" width="11.712962962963" customWidth="true"/>
-    <col min="6" max="6" width="9.71296296296296" customWidth="true"/>
-    <col min="7" max="7" width="44.712962962963" customWidth="true"/>
-    <col min="8" max="8" width="32.4259259259259" customWidth="true"/>
-    <col min="9" max="9" width="21.712962962963" customWidth="true"/>
-    <col min="10" max="10" width="9.28703703703704" customWidth="true"/>
-    <col min="12" max="12" width="22.9444444444444" customWidth="true"/>
+    <col min="2" max="2" width="11.1428571428571" customWidth="true"/>
+    <col min="3" max="3" width="14.1428571428571" customWidth="true"/>
+    <col min="4" max="4" width="20.1428571428571" customWidth="true"/>
+    <col min="5" max="5" width="11.7142857142857" customWidth="true"/>
+    <col min="6" max="6" width="9.71428571428571" customWidth="true"/>
+    <col min="7" max="7" width="44.7142857142857" customWidth="true"/>
+    <col min="8" max="8" width="32.4285714285714" customWidth="true"/>
+    <col min="9" max="9" width="21.7142857142857" customWidth="true"/>
+    <col min="10" max="10" width="9.28571428571429" customWidth="true"/>
+    <col min="12" max="12" width="22.9428571428571" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1275,7 +1272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:11">
       <c r="A6" s="1"/>
       <c r="D6" t="s">
         <v>26</v>
@@ -1293,46 +1290,40 @@
       <c r="K6" t="b">
         <v>1</v>
       </c>
-      <c r="L6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="1"/>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" t="s">
         <v>31</v>
-      </c>
-      <c r="H7" t="s">
-        <v>32</v>
       </c>
       <c r="I7" s="3"/>
       <c r="K7" t="b">
         <v>1</v>
-      </c>
-      <c r="L7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1"/>
       <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" t="s">
         <v>33</v>
       </c>
-      <c r="E8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>34</v>
-      </c>
-      <c r="H8" t="s">
-        <v>35</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" t="b">
@@ -1341,20 +1332,20 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
         <v>36</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>37</v>
-      </c>
-      <c r="E9" t="s">
-        <v>38</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" t="s">
         <v>39</v>
-      </c>
-      <c r="H9" t="s">
-        <v>40</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" t="b">
@@ -1366,19 +1357,19 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s">
         <v>41</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
         <v>42</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>43</v>
-      </c>
-      <c r="H10" t="s">
-        <v>44</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" t="b">
@@ -1390,19 +1381,19 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
       </c>
       <c r="G11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" t="s">
         <v>46</v>
-      </c>
-      <c r="H11" t="s">
-        <v>47</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" t="b">
@@ -1476,10 +1467,10 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="13.2" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="true"/>
-    <col min="2" max="2" width="12.287037037037" customWidth="true"/>
+    <col min="2" max="2" width="12.2857142857143" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1487,7 +1478,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
@@ -1511,33 +1502,33 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="13.2" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="true"/>
-    <col min="2" max="2" width="20.4259259259259" customWidth="true"/>
-    <col min="3" max="3" width="23.287037037037" customWidth="true"/>
+    <col min="2" max="2" width="20.4285714285714" customWidth="true"/>
+    <col min="3" max="3" width="23.2857142857143" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" t="s">
         <v>50</v>
-      </c>
-      <c r="C1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
         <v>52</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>53</v>
-      </c>
-      <c r="C2" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add more validations to Household Form, set non-required gps coordinates
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/household_form.xlsx
+++ b/app/src/main/res/raw/household_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26265" windowHeight="9390" tabRatio="500"/>
+    <workbookView windowWidth="28800" windowHeight="12330" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -194,10 +194,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -219,6 +219,90 @@
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -230,28 +314,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
@@ -267,98 +329,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -367,187 +367,193 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -558,26 +564,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -605,17 +591,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -637,166 +623,186 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -806,12 +812,13 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1134,8 +1141,8 @@
   <sheetPr/>
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -1194,7 +1201,7 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="5" t="s">
         <v>13</v>
       </c>
       <c r="O1" t="s">
@@ -1354,9 +1361,7 @@
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-      <c r="L8" t="b">
-        <v>1</v>
-      </c>
+      <c r="L8" s="3"/>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
@@ -1447,8 +1452,8 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="1"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="1"/>

</xml_diff>

<commit_message>
- Add custom title for Region Registration Form - Allow editing a region by clicking on Add after selecting the region
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/household_form.xlsx
+++ b/app/src/main/res/raw/household_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27795" windowHeight="12270" tabRatio="500"/>
+    <workbookView windowWidth="13170" windowHeight="7050" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -248,10 +248,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -259,6 +259,104 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -270,36 +368,37 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -312,105 +411,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -427,187 +427,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -698,6 +698,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -713,11 +722,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -729,15 +759,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -757,36 +778,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -795,151 +786,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1296,7 +1296,7 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A9" sqref="$A9:$XFD12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -1369,7 +1369,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -1393,9 +1393,6 @@
       <c r="M2" t="b">
         <v>1</v>
       </c>
-      <c r="N2" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
@@ -1607,16 +1604,12 @@
       <c r="A11" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
       <c r="H11" s="4" t="s">
         <v>61</v>
       </c>
@@ -1628,12 +1621,9 @@
       </c>
       <c r="K11" s="14"/>
       <c r="L11" s="14"/>
-      <c r="M11" s="4"/>
       <c r="N11" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
       <c r="Q11" s="4" t="b">
         <v>1</v>
       </c>

</xml_diff>